<commit_message>
updated ui and tests
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -25,10 +25,10 @@
     <t>balance</t>
   </si>
   <si>
-    <t>U46ApQuCVHXhbt0tn2eW</t>
-  </si>
-  <si>
-    <t>shKIGGYEaRZL57kmOVnI</t>
+    <t>dmxQwKymKD3FrUgJHgCr</t>
+  </si>
+  <si>
+    <t>wYfhX0ordSBl1agNeVgm</t>
   </si>
   <si>
     <t>John Don</t>

</xml_diff>

<commit_message>
edits for the doc
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -25,10 +25,10 @@
     <t>balance</t>
   </si>
   <si>
-    <t>dmxQwKymKD3FrUgJHgCr</t>
-  </si>
-  <si>
-    <t>wYfhX0ordSBl1agNeVgm</t>
+    <t>L5FzvRYyZyRtrIofAyYS</t>
+  </si>
+  <si>
+    <t>wMVY6Ls9uzob9kch569W</t>
   </si>
   <si>
     <t>John Don</t>

</xml_diff>